<commit_message>
Inputs and Outputs get written to a log file and added more data to spreadsheet
</commit_message>
<xml_diff>
--- a/Throughput Data.xlsx
+++ b/Throughput Data.xlsx
@@ -5,22 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinho/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinho/Desktop/Cilent_Socket_Server-master/Cilent_Socket_Server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA258B4-F965-A445-B2A9-5D8248E4134A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7639FC-AA1A-ED4D-A87F-C3B086006CB6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" activeTab="1" xr2:uid="{F8F23A02-DAE1-874A-A8C8-1BA47E20EF2D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" xr2:uid="{F8F23A02-DAE1-874A-A8C8-1BA47E20EF2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Remote Shell Throughput" sheetId="1" r:id="rId1"/>
     <sheet name="wget Throughput" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'wget Throughput'!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'wget Throughput'!$A$2:$A$51</definedName>
-  </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Throughput (KB/s)</t>
   </si>
@@ -48,6 +44,12 @@
   </si>
   <si>
     <t>Number of Runs</t>
+  </si>
+  <si>
+    <t>Minimum Response Time (ms)</t>
+  </si>
+  <si>
+    <t>Response Time (ms)</t>
   </si>
 </sst>
 </file>
@@ -2194,16 +2196,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>254000</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2569,305 +2571,466 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DA7BE2-6C62-1F4A-974A-098768A5677A}">
-  <dimension ref="A1:R51"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>2000</v>
       </c>
-      <c r="R2" s="4">
+      <c r="B2" s="3">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="P2" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>5764.7058820000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>13363.636364</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="B4" s="3">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>21777.777778</v>
       </c>
-      <c r="R5" s="3">
+      <c r="B5" s="3">
+        <v>2.7E-2</v>
+      </c>
+      <c r="P5" s="3">
         <f>MIN(A2:A51)</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>18148.148148</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>14700</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="B7" s="3">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="P7" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>16333.333333</v>
       </c>
-      <c r="R8" s="3">
+      <c r="B8" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="P8" s="3">
         <f>MAX(A2:A51)</f>
         <v>218950</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>28000</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>33923.076923000001</v>
       </c>
-      <c r="R10" s="2" t="s">
+      <c r="B10" s="3">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="P10" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>19215.686275</v>
       </c>
-      <c r="R11" s="3">
+      <c r="B11" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="P11" s="3">
         <f>AVERAGE(A2:A51)</f>
         <v>94175.363653480017</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>44916.666666999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>56000</v>
       </c>
-      <c r="R13" s="2" t="s">
+      <c r="B13" s="3">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="P13" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>84933.333333000002</v>
       </c>
-      <c r="R14" s="3">
+      <c r="B14" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="P14" s="3">
         <f>STDEV(A2:A51)</f>
         <v>56825.509507606803</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>54880</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <v>6.2E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>54444.444444000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>104533.333333</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="P17" s="3">
+        <f>MIN(B2:B51)</f>
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>44351.351350999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>99000</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>50531.914894000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>125210.526316</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>73147.058824000007</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>103400</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>95821.428570999997</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>63139.534884000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
+        <v>3.1E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>104185.18518499999</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>137428.571429</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>92468.75</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28" s="3">
+        <v>3.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>152850</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29" s="3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>80897.435897000003</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>130120</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31" s="3">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>139625</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" s="3">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>137960</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" s="3">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>168904.76190499999</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" s="3">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>101250</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" s="3">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>149720</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" s="3">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>112970.588235</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37" s="3">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>207315.78947399999</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38" s="3">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>182363.63636400001</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39" s="3">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>97857.142856999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40" s="3">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>76509.090909000006</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>215300</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42" s="3">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>218950</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43" s="3">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>89540</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44" s="3">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>96808.510638000007</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45" s="3">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>118538.461538</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46" s="3">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>100446.808511</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47" s="3">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>117536.585366</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" s="3">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>169551.72413799999</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" s="3">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>172068.965517</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" s="3">
+        <v>4.1000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>110065.217391</v>
+      </c>
+      <c r="B51" s="3">
+        <v>3.5999999999999997E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2881,7 +3044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C1F8D4-6921-E44F-822F-8FC5C2113464}">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>

</xml_diff>